<commit_message>
Commit finished simulations and data analysis
</commit_message>
<xml_diff>
--- a/CS1538 Group Project Data.xlsx
+++ b/CS1538 Group Project Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="44">
   <si>
     <t>Printer Usa0e</t>
   </si>
@@ -147,12 +147,18 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t>23.6 avg per hour</t>
+  </si>
+  <si>
+    <t>6.4 per hour</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -160,6 +166,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -327,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -375,6 +387,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,11 +784,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-30"/>
-        <c:axId val="2085316560"/>
-        <c:axId val="2085318736"/>
+        <c:axId val="-1893336800"/>
+        <c:axId val="-1893330272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2085316560"/>
+        <c:axId val="-1893336800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085318736"/>
+        <c:crossAx val="-1893330272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -817,7 +830,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085318736"/>
+        <c:axId val="-1893330272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +875,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085316560"/>
+        <c:crossAx val="-1893336800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -2244,11 +2257,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085320912"/>
-        <c:axId val="2085319280"/>
+        <c:axId val="-1893324832"/>
+        <c:axId val="-1893334624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085320912"/>
+        <c:axId val="-1893324832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2323,14 +2336,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085319280"/>
+        <c:crossAx val="-1893334624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2085319280"/>
+        <c:axId val="-1893334624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="36"/>
@@ -2405,7 +2418,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085320912"/>
+        <c:crossAx val="-1893324832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2803,11 +2816,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2085322544"/>
-        <c:axId val="2085326896"/>
+        <c:axId val="-1893324288"/>
+        <c:axId val="-1893327008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2085322544"/>
+        <c:axId val="-1893324288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,7 +2854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085326896"/>
+        <c:crossAx val="-1893327008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2849,7 +2862,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085326896"/>
+        <c:axId val="-1893327008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2085322544"/>
+        <c:crossAx val="-1893324288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -4352,8 +4365,8 @@
   </sheetPr>
   <dimension ref="A1:IV1039"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7423,8 +7436,12 @@
       <c r="D169" s="15"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
-      <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
+      <c r="G169" s="2">
+        <v>118</v>
+      </c>
+      <c r="H169" s="2">
+        <v>32</v>
+      </c>
       <c r="I169" s="2"/>
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
@@ -7440,8 +7457,12 @@
       <c r="D170" s="15"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
-      <c r="G170" s="2"/>
-      <c r="H170" s="2"/>
+      <c r="G170" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H170" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="I170" s="2"/>
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>

</xml_diff>